<commit_message>
Input for small cities (this&next)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/input prep/input.xlsx
+++ b/migforecasting/less100/input prep/input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>Бокситогорский МР</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,6 +1173,306 @@
         <v>-550</v>
       </c>
     </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="2">
+        <v>50.756</v>
+      </c>
+      <c r="D15" s="2">
+        <v>9.8539999999999992</v>
+      </c>
+      <c r="E15" s="2">
+        <v>497.40879999999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>33918.400000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>30.7</v>
+      </c>
+      <c r="H15" s="2">
+        <v>894.31299999999999</v>
+      </c>
+      <c r="I15" s="2">
+        <v>22261.996999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>196.75200000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1640.018</v>
+      </c>
+      <c r="M15" s="2">
+        <v>14.432</v>
+      </c>
+      <c r="N15" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O15" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P15" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C16" s="2">
+        <v>51.298000000000002</v>
+      </c>
+      <c r="D16" s="2">
+        <v>9.8369999999999997</v>
+      </c>
+      <c r="E16" s="2">
+        <v>559.14819999999997</v>
+      </c>
+      <c r="F16" s="2">
+        <v>31340.5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1381.8050000000001</v>
+      </c>
+      <c r="I16" s="2">
+        <v>19849.96</v>
+      </c>
+      <c r="J16" s="2">
+        <v>159.67099999999999</v>
+      </c>
+      <c r="K16" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1348.8230000000001</v>
+      </c>
+      <c r="M16" s="2">
+        <v>17.542000000000002</v>
+      </c>
+      <c r="N16" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O16" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P16" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C17" s="2">
+        <v>51.941000000000003</v>
+      </c>
+      <c r="D17" s="2">
+        <v>9.9879999999999995</v>
+      </c>
+      <c r="E17" s="2">
+        <v>597.32150000000001</v>
+      </c>
+      <c r="F17" s="2">
+        <v>28366.2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H17" s="2">
+        <v>814.22699999999998</v>
+      </c>
+      <c r="I17" s="2">
+        <v>17254.972000000002</v>
+      </c>
+      <c r="J17" s="2">
+        <v>173.51900000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="L17" s="2">
+        <v>967.63780000000008</v>
+      </c>
+      <c r="M17" s="2">
+        <v>16.149000000000001</v>
+      </c>
+      <c r="N17" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O17" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P17" s="2">
+        <v>-257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C18" s="2">
+        <v>52.34</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10.254</v>
+      </c>
+      <c r="E18" s="2">
+        <v>711.82400000000007</v>
+      </c>
+      <c r="F18" s="2">
+        <v>25409.8</v>
+      </c>
+      <c r="G18" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H18" s="2">
+        <v>691.16099999999994</v>
+      </c>
+      <c r="I18" s="2">
+        <v>17653.433000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>85.984999999999999</v>
+      </c>
+      <c r="K18" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L18" s="2">
+        <v>821.76700000000005</v>
+      </c>
+      <c r="M18" s="2">
+        <v>24.484999999999999</v>
+      </c>
+      <c r="N18" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O18" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P18" s="2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C19" s="2">
+        <v>52.956000000000003</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10.59</v>
+      </c>
+      <c r="E19" s="2">
+        <v>751.97519999999997</v>
+      </c>
+      <c r="F19" s="2">
+        <v>23164</v>
+      </c>
+      <c r="G19" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H19" s="2">
+        <v>955.6</v>
+      </c>
+      <c r="I19" s="2">
+        <v>16316.396500000001</v>
+      </c>
+      <c r="J19" s="2">
+        <v>230.62899999999999</v>
+      </c>
+      <c r="K19" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>714.0385</v>
+      </c>
+      <c r="M19" s="2">
+        <v>32.409999999999997</v>
+      </c>
+      <c r="N19" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O19" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P19" s="2">
+        <v>-76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2011</v>
+      </c>
+      <c r="C20" s="2">
+        <v>53.338000000000001</v>
+      </c>
+      <c r="D20" s="2">
+        <v>11.303000000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1002.7544</v>
+      </c>
+      <c r="F20" s="2">
+        <v>20279</v>
+      </c>
+      <c r="G20" s="2">
+        <v>36.43</v>
+      </c>
+      <c r="H20" s="2">
+        <v>577.28300000000002</v>
+      </c>
+      <c r="I20" s="2">
+        <v>15980.2601</v>
+      </c>
+      <c r="J20" s="2">
+        <v>309.06599999999997</v>
+      </c>
+      <c r="K20" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="L20" s="2">
+        <v>633.4</v>
+      </c>
+      <c r="M20" s="2">
+        <v>29.247</v>
+      </c>
+      <c r="N20" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O20" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P20" s="2">
+        <v>-150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>